<commit_message>
feat nova estrutura eixos + gravar regra no banco
</commit_message>
<xml_diff>
--- a/dados/base_iniciativas_resumos_sei.xlsx
+++ b/dados/base_iniciativas_resumos_sei.xlsx
@@ -1,37 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icmbioe5.sharepoint.com/sites/IPS/Documentos Compartilhados/repo_cocam/Planejamento 2025/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E4F8135-E706-4703-80F8-BA7170FE46A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="6060" windowWidth="38640" windowHeight="15720" xr2:uid="{420C2663-29A7-4A25-A2A1-A8DF0660B4B6}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -788,7 +766,7 @@
     <t>Coordenação de Pesquisa e Gestão da Informação sobre Biodiversidade - COPEG</t>
   </si>
   <si>
-    <t>COPEG</t>
+    <t>CGPEQ</t>
   </si>
   <si>
     <t>Programa de Fomento e Apoio às Pesquisas Estratégicas para o Manejo das Unidades de Conservação Federais.</t>
@@ -1259,12 +1237,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1289,34 +1268,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1343,116 +1325,82 @@
         <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1464,540 +1412,563 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53BC45C6-619A-4F43-A6AB-847C4F1AD584}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" hidden="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" hidden="1">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" hidden="1">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" hidden="1">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" hidden="1">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" hidden="1">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" hidden="1">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" hidden="1">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" hidden="1">
+      <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="1319.25">
+      <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" hidden="1">
+      <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" hidden="1">
+      <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix page 2 cadastros
</commit_message>
<xml_diff>
--- a/dados/base_iniciativas_resumos_sei.xlsx
+++ b/dados/base_iniciativas_resumos_sei.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmagi\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4F7AC6-0AED-4FDD-BC66-E9471DC62E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="4575" yWindow="1050" windowWidth="19695" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>Diretoria</t>
   </si>
@@ -1233,12 +1239,14 @@
 https://www.icmbio.gov.br/cbc/images/stories/Publica%C3%A7%C3%B5es/restaura%C3 
 %A7%C3%A3o/Guia-de-Restauracao-Ecologica_digital.pdf</t>
   </si>
+  <si>
+    <t>id_resumo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1268,23 +1276,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1295,10 +1300,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1336,71 +1341,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1428,7 +1433,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1451,11 +1456,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1464,13 +1469,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1480,7 +1485,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1489,7 +1494,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1498,7 +1503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1506,10 +1511,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1574,397 +1579,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="140.5703125" customWidth="1"/>
+    <col min="7" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" hidden="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" hidden="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" hidden="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" hidden="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" hidden="1">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" hidden="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" hidden="1">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" hidden="1">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" hidden="1">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="1319.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" hidden="1">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" hidden="1">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" t="s">
         <v>103</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: new table db : tf_distribuicao_elegiveis; upload update new files ; tabela populada
</commit_message>
<xml_diff>
--- a/dados/base_iniciativas_resumos_sei.xlsx
+++ b/dados/base_iniciativas_resumos_sei.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmagi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4F7AC6-0AED-4FDD-BC66-E9471DC62E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F454A2D-2A4C-4B34-A743-DB268A518C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="1050" windowWidth="19695" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-10875" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>Diretoria</t>
   </si>
@@ -59,9 +72,6 @@
   </si>
   <si>
     <t>Coordenação de Fiscalização - COFIS</t>
-  </si>
-  <si>
-    <t>COFIS</t>
   </si>
   <si>
     <t>Proposta de captação de recursos da compensação ambiental para o fortalecimento da estratégia e 
@@ -181,9 +191,6 @@
   </si>
   <si>
     <t>Coordenação de Manejo Integrado do Fogo - CMIF</t>
-  </si>
-  <si>
-    <t>CMIF</t>
   </si>
   <si>
     <t>Ações de Manejo Integrado do Fogo para as UCs.</t>
@@ -342,9 +349,6 @@
     <t>Coordenação de Planos de Manejo de Unidades de Conservação - COMAN</t>
   </si>
   <si>
-    <t>COMAN</t>
-  </si>
-  <si>
     <t>Dotar as UCs Federais Com Planos de Manejo Atuais e Adequados à IN 07/17 do ICMBIO</t>
   </si>
   <si>
@@ -387,9 +391,6 @@
   </si>
   <si>
     <t>Coordenação de Planejamento, Estruturação da Visitação e do Ecoturismo - COEST</t>
-  </si>
-  <si>
-    <t>COEST</t>
   </si>
   <si>
     <t>Implementar as unidades de conservação federais na gestão do uso público.</t>
@@ -446,9 +447,6 @@
     <t>Coordenação Geral de Gestão Socioambiental - CGSAM</t>
   </si>
   <si>
-    <t>CGSAM</t>
-  </si>
-  <si>
     <t>Fortalecendo a participação social nas Ações de Gestão Socioambiental nas UCs federais.</t>
   </si>
   <si>
@@ -515,9 +513,6 @@
   </si>
   <si>
     <t>Coordenação-Geral de Populações Tradicionais - CGPT</t>
-  </si>
-  <si>
-    <t>CGPT</t>
   </si>
   <si>
     <t xml:space="preserve">Fortalecimento das economias da socio biodiversidade e da 
@@ -625,9 +620,6 @@
   </si>
   <si>
     <t>Coordenação de Monitoramento da Biodiversidade - COMOB</t>
-  </si>
-  <si>
-    <t>COMOB</t>
   </si>
   <si>
     <t xml:space="preserve">Proposta de captação de recursos da compensação ambiental 
@@ -730,9 +722,6 @@
     <t>Coordenação-Geral de Consolidação Territorial - CGTER</t>
   </si>
   <si>
-    <t>CGTER</t>
-  </si>
-  <si>
     <t>Fortalecimento da Regularização Fundiária nas Unidades de Conservação de Uso Sustentável.</t>
   </si>
   <si>
@@ -770,9 +759,6 @@
   </si>
   <si>
     <t>Coordenação de Pesquisa e Gestão da Informação sobre Biodiversidade - COPEG</t>
-  </si>
-  <si>
-    <t>CGPEQ</t>
   </si>
   <si>
     <t>Programa de Fomento e Apoio às Pesquisas Estratégicas para o Manejo das Unidades de Conservação Federais.</t>
@@ -972,9 +958,6 @@
     <t>Coordenação-Geral de Estratégias para Conservação - CGCON</t>
   </si>
   <si>
-    <t>CGCON</t>
-  </si>
-  <si>
     <t>Implementação de ações estratégicas para a conservação e manejo da biodiversidade nas UCs federais.</t>
   </si>
   <si>
@@ -1128,9 +1111,6 @@
     <t>Centro Nacional de Pesquisa e Conservação da Biodiversidade do Cerrado e Restauração Ecológica - CBC</t>
   </si>
   <si>
-    <t>CBC</t>
-  </si>
-  <si>
     <t>Ações estratégicas de restauração ecológica de áreas degradadas em UC.</t>
   </si>
   <si>
@@ -1241,6 +1221,15 @@
   </si>
   <si>
     <t>id_resumo</t>
+  </si>
+  <si>
+    <t>DIMAN</t>
+  </si>
+  <si>
+    <t>DISAT</t>
+  </si>
+  <si>
+    <t>DIBIO</t>
   </si>
 </sst>
 </file>
@@ -1585,13 +1574,13 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="91" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="140.5703125" customWidth="1"/>
@@ -1612,7 +1601,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1644,28 +1633,28 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1676,31 +1665,31 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1708,34 +1697,34 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="E4">
         <v>6</v>
       </c>
       <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1743,261 +1732,261 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="E6">
         <v>13</v>
       </c>
       <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
         <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E9">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
         <v>97</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="I12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="K12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>